<commit_message>
commit a little bit change
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\Desktop\IMI Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nan Wilshere\Desktop\imi-document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>Table Name</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>customers</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -767,7 +770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -787,7 +790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -807,7 +810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -824,7 +827,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>24</v>
       </c>
@@ -839,6 +842,11 @@
       </c>
       <c r="H21" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit data dictionary of vendors table
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
   <si>
     <t>Table Name</t>
   </si>
@@ -140,7 +140,49 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>customers</t>
+    <t>vendors</t>
+  </si>
+  <si>
+    <t>vendor_type_id</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>cantact_title</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
@@ -474,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -770,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -790,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -810,7 +852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -827,7 +869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>24</v>
       </c>
@@ -844,9 +886,306 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>9999999999</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>9999999999</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>9999999999</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>9999999999</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit completed vendor design table
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nan Wilshere\Desktop\imi-document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\Desktop\imi-document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="58">
   <si>
     <t>Table Name</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>country</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>N/a</t>
+  </si>
+  <si>
+    <t>branch_id</t>
+  </si>
+  <si>
+    <t>Unsigned</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -236,6 +251,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,15 +548,16 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="7" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="12" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,32 +570,35 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -583,142 +608,151 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
         <v>9999999999</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
         <v>9999999999</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
         <v>9999999999</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="H9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -728,165 +762,177 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13">
         <v>9999999999</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14">
         <v>9999999999</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
         <v>36</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18">
         <v>9999999999</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19">
         <v>9999999999</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="H20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -896,295 +942,369 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23">
         <v>9999999999</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="H23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>39</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24">
         <v>9999999999</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="H24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
         <v>36</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>9999999999</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>41</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>20</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>25</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F38" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="H38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>21</v>
-      </c>
-      <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38">
-        <v>9999999999</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>22</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39">
         <v>9999999999</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40">
+        <v>9999999999</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>23</v>
-      </c>
-      <c r="D40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>24</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="H41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit account type table
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="63">
   <si>
     <t>Table Name</t>
   </si>
@@ -198,6 +198,21 @@
   </si>
   <si>
     <t>Unsigned</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>min_code</t>
+  </si>
+  <si>
+    <t>max_code</t>
+  </si>
+  <si>
+    <t>enum{'ASSETS','EQUITY','EXPENSES','LIABILITIES','REVENUE'}</t>
   </si>
 </sst>
 </file>
@@ -537,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +563,7 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" customWidth="1"/>
@@ -1126,7 +1141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>48</v>
       </c>
@@ -1160,7 +1175,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>49</v>
       </c>
@@ -1177,7 +1192,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>46</v>
       </c>
@@ -1194,7 +1209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>21</v>
       </c>
@@ -1251,7 +1266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>22</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>24</v>
       </c>
@@ -1305,6 +1320,185 @@
         <v>31</v>
       </c>
       <c r="I42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44">
+        <v>9999999999</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47">
+        <v>9999999999</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>9999999999</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50">
+        <v>9999999999</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51">
+        <v>9999999999</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit update structure table
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="64">
   <si>
     <t>Table Name</t>
   </si>
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,12 +770,35 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>9999999999</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>57</v>
-      </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -793,86 +816,86 @@
         <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14">
-        <v>9999999999</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>9999999999</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>62</v>
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -895,19 +918,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <v>9999999999</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>30</v>
@@ -916,14 +933,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -933,30 +950,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>9999999999</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -974,7 +997,10 @@
         <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1131,12 +1157,61 @@
         <v>34</v>
       </c>
     </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>9999999999</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>9999999999</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
@@ -1154,64 +1229,46 @@
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="K35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36">
-        <v>9999999999</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>47</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J36" t="s">
-        <v>33</v>
-      </c>
-      <c r="K36" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37">
-        <v>9999999999</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" t="s">
-        <v>33</v>
-      </c>
-      <c r="K37" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="I37" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
         <v>26</v>
@@ -1220,15 +1277,18 @@
         <v>47</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F39" t="s">
         <v>47</v>
@@ -1242,10 +1302,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F40" t="s">
         <v>47</v>
@@ -1259,96 +1319,96 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" t="s">
-        <v>47</v>
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>9999999999</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I41" t="s">
         <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" t="s">
-        <v>47</v>
+        <v>14</v>
+      </c>
+      <c r="F42">
+        <v>9999999999</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I42" t="s">
         <v>34</v>
+      </c>
+      <c r="J42" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43">
-        <v>9999999999</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>47</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
-      </c>
-      <c r="J43" t="s">
-        <v>33</v>
-      </c>
-      <c r="K43" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44">
-        <v>9999999999</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>47</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I44" t="s">
         <v>34</v>
-      </c>
-      <c r="J44" t="s">
-        <v>33</v>
-      </c>
-      <c r="K44" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F45" t="s">
         <v>47</v>
@@ -1362,10 +1422,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F46" t="s">
         <v>47</v>
@@ -1379,30 +1439,36 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F47" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" t="s">
-        <v>47</v>
+        <v>14</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>9999999999</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>30</v>
@@ -1413,36 +1479,36 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>9999999999</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>62</v>
+        <v>30</v>
+      </c>
+      <c r="I49" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50">
-        <v>9999999999</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>30</v>
@@ -1451,21 +1517,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51">
-        <v>9999999999</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>30</v>
@@ -1474,58 +1534,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" t="s">
-        <v>31</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53">
+        <v>9999999999</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>52</v>
-      </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55">
-        <v>9999999999</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="F55" t="s">
+        <v>29</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>16</v>
@@ -1533,10 +1584,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56">
+        <v>9999999999</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>16</v>
@@ -1544,13 +1604,19 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>9999999999</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>16</v>
@@ -1558,27 +1624,24 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58">
-        <v>9999999999</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D59" t="s">
         <v>14</v>
@@ -1593,41 +1656,41 @@
         <v>15</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I59" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
-      </c>
-      <c r="F60" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60">
+        <v>9999999999</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>62</v>
+        <v>30</v>
+      </c>
+      <c r="I60" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61">
-        <v>9999999999</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>30</v>
@@ -1638,52 +1701,15 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62">
-        <v>9999999999</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I62" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" t="s">
-        <v>27</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I63" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-      <c r="D64" t="s">
-        <v>27</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I64" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit update reorder field table
</commit_message>
<xml_diff>
--- a/IMI Data Dictionary.xlsx
+++ b/IMI Data Dictionary.xlsx
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,39 +1396,27 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38">
-        <v>9999999999</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J38" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>16</v>
@@ -1436,38 +1424,50 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I40" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>44</v>
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>9999999999</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I41" t="s">
         <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -1488,38 +1488,29 @@
         <v>33</v>
       </c>
       <c r="K42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43">
-        <v>9999999999</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>44</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
-      </c>
-      <c r="J43" t="s">
-        <v>33</v>
-      </c>
-      <c r="K43" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
         <v>43</v>
@@ -1536,10 +1527,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F45" t="s">
         <v>44</v>
@@ -1553,7 +1544,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
         <v>25</v>
@@ -1570,19 +1561,28 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" t="s">
-        <v>44</v>
+        <v>14</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47">
+        <v>9999999999</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="J47" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1953,53 +1953,44 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F68">
-        <v>9999999999</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F68" t="s">
+        <v>28</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J68" t="s">
-        <v>33</v>
-      </c>
-      <c r="K68" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D69" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I69" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>30</v>
@@ -2010,7 +2001,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D71" t="s">
         <v>43</v>
@@ -2027,10 +2018,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F72" t="s">
         <v>46</v>
@@ -2044,10 +2035,10 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D73" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F73" t="s">
         <v>46</v>
@@ -2061,24 +2052,36 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D74" t="s">
-        <v>43</v>
-      </c>
-      <c r="F74" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74">
+        <v>9999999999</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I74" t="s">
         <v>34</v>
+      </c>
+      <c r="J74" t="s">
+        <v>33</v>
+      </c>
+      <c r="K74" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D75" t="s">
         <v>14</v>
@@ -2102,41 +2105,29 @@
         <v>33</v>
       </c>
       <c r="K75" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F76">
-        <v>9999999999</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F76" t="s">
+        <v>46</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I76" t="s">
         <v>34</v>
-      </c>
-      <c r="J76" t="s">
-        <v>33</v>
-      </c>
-      <c r="K76" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D77" t="s">
         <v>43</v>
@@ -2153,10 +2144,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F78" t="s">
         <v>46</v>
@@ -2170,7 +2161,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D79" t="s">
         <v>25</v>
@@ -2187,19 +2178,28 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D80" t="s">
-        <v>25</v>
-      </c>
-      <c r="F80" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F80">
+        <v>9999999999</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I80" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="J80" t="s">
+        <v>33</v>
+      </c>
+      <c r="K80" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2407,42 +2407,27 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F92">
-        <v>9999999999</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F92" t="s">
+        <v>28</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" t="s">
-        <v>34</v>
-      </c>
-      <c r="J92" t="s">
-        <v>33</v>
-      </c>
-      <c r="K92" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D93" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F93" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>16</v>
@@ -2450,13 +2435,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D94" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>16</v>
@@ -2464,7 +2449,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D95" t="s">
         <v>43</v>
@@ -2473,29 +2458,44 @@
         <v>46</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I95" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D96" t="s">
-        <v>43</v>
-      </c>
-      <c r="F96" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F96">
+        <v>9999999999</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I96" t="s">
         <v>34</v>
+      </c>
+      <c r="J96" t="s">
+        <v>33</v>
+      </c>
+      <c r="K96" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D97" t="s">
         <v>14</v>
@@ -2519,41 +2519,29 @@
         <v>33</v>
       </c>
       <c r="K97" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F98">
-        <v>9999999999</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F98" t="s">
+        <v>46</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I98" t="s">
         <v>34</v>
-      </c>
-      <c r="J98" t="s">
-        <v>33</v>
-      </c>
-      <c r="K98" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D99" t="s">
         <v>43</v>
@@ -2570,10 +2558,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D100" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F100" t="s">
         <v>46</v>
@@ -2587,7 +2575,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D101" t="s">
         <v>25</v>
@@ -2604,19 +2592,28 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D102" t="s">
-        <v>25</v>
-      </c>
-      <c r="F102" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F102">
+        <v>9999999999</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I102" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="J102" t="s">
+        <v>33</v>
+      </c>
+      <c r="K102" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -2638,7 +2635,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D104" t="s">
         <v>14</v>
@@ -2653,13 +2650,16 @@
         <v>15</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I104" t="s">
+        <v>34</v>
       </c>
       <c r="J104" t="s">
         <v>33</v>
       </c>
       <c r="K104" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -2836,39 +2836,27 @@
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D115" t="s">
-        <v>14</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F115">
-        <v>9999999999</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F115" t="s">
+        <v>28</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J115" t="s">
-        <v>33</v>
-      </c>
-      <c r="K115" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D116" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F116" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>16</v>
@@ -2876,7 +2864,7 @@
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D117" t="s">
         <v>68</v>
@@ -2885,12 +2873,12 @@
         <v>69</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D118" t="s">
         <v>68</v>
@@ -2904,7 +2892,7 @@
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D119" t="s">
         <v>68</v>
@@ -2918,7 +2906,7 @@
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D120" t="s">
         <v>68</v>
@@ -2932,21 +2920,27 @@
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D121" t="s">
-        <v>68</v>
-      </c>
-      <c r="F121" t="s">
-        <v>69</v>
+        <v>14</v>
+      </c>
+      <c r="F121">
+        <v>9999999999</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I121" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D122" t="s">
         <v>14</v>
@@ -2966,27 +2960,21 @@
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="D123" t="s">
-        <v>14</v>
-      </c>
-      <c r="F123">
-        <v>9999999999</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F123" t="s">
+        <v>46</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I123" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D124" t="s">
         <v>43</v>
@@ -2995,29 +2983,44 @@
         <v>46</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I124" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D125" t="s">
-        <v>43</v>
-      </c>
-      <c r="F125" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F125">
+        <v>9999999999</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I125" t="s">
         <v>34</v>
+      </c>
+      <c r="J125" t="s">
+        <v>33</v>
+      </c>
+      <c r="K125" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D126" t="s">
         <v>14</v>
@@ -3041,41 +3044,29 @@
         <v>33</v>
       </c>
       <c r="K126" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D127" t="s">
-        <v>14</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F127">
-        <v>9999999999</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F127" t="s">
+        <v>46</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I127" t="s">
         <v>34</v>
-      </c>
-      <c r="J127" t="s">
-        <v>33</v>
-      </c>
-      <c r="K127" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D128" t="s">
         <v>43</v>
@@ -3092,10 +3083,10 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D129" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F129" t="s">
         <v>46</v>
@@ -3109,7 +3100,7 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D130" t="s">
         <v>25</v>
@@ -3126,19 +3117,28 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D131" t="s">
-        <v>25</v>
-      </c>
-      <c r="F131" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F131">
+        <v>9999999999</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I131" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="J131" t="s">
+        <v>33</v>
+      </c>
+      <c r="K131" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
@@ -3333,33 +3333,24 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="D142" t="s">
-        <v>14</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F142">
-        <v>9999999999</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J142" t="s">
-        <v>33</v>
-      </c>
-      <c r="K142" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D143" t="s">
         <v>91</v>
@@ -3376,16 +3367,16 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D144" t="s">
-        <v>91</v>
-      </c>
-      <c r="F144" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G144" s="6" t="s">
-        <v>93</v>
+        <v>14</v>
+      </c>
+      <c r="F144">
+        <v>9999999999</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H144" s="2" t="s">
         <v>16</v>
@@ -3393,71 +3384,80 @@
     </row>
     <row r="145" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
-      </c>
-      <c r="F145">
-        <v>9999999999</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F145" t="s">
+        <v>46</v>
+      </c>
+      <c r="G145" s="1"/>
       <c r="H145" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="I145" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D146" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="F146" t="s">
         <v>46</v>
       </c>
-      <c r="G146" s="1"/>
       <c r="H146" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I146" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="I146" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="D147" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="F147" t="s">
         <v>46</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I147" s="3">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="I147" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D148" t="s">
-        <v>25</v>
-      </c>
-      <c r="F148" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F148">
+        <v>9999999999</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I148" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="J148" t="s">
+        <v>33</v>
+      </c>
+      <c r="K148" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>